<commit_message>
practicas pre y post parciales
</commit_message>
<xml_diff>
--- a/informaticaAplicada/laboratorio/Excel/02 - Fletes Carlitos.xlsx
+++ b/informaticaAplicada/laboratorio/Excel/02 - Fletes Carlitos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgraf\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2ec1f9f747361b47/Escritorio/Mis archivos/Practicas de clases y primeros proyectos/informaticaAplicada/Laboratorio/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A0BC33-2769-4938-9723-8E93AF0D5E90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="263" documentId="13_ncr:1_{54A0BC33-2769-4938-9723-8E93AF0D5E90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F1BAD60-0621-4927-ACC7-109F2AEFB11E}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{62756508-513B-423E-9AD5-61F1B99F94A7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{62756508-513B-423E-9AD5-61F1B99F94A7}"/>
   </bookViews>
   <sheets>
     <sheet name="FLETES CARLITOS" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'FLETES CARLITOS'!$A$1:$K$28</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'FLETES CARLITOS'!$A$1:$L$28</definedName>
     <definedName name="nota" localSheetId="0">'FLETES CARLITOS'!#REF!</definedName>
     <definedName name="nota">'[1]FLETES CARLITOS'!$U$5:$AE$6</definedName>
   </definedNames>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
   <si>
     <t>Nro Envío</t>
   </si>
@@ -309,6 +309,12 @@
   <si>
     <t>Fecha de recepcion</t>
   </si>
+  <si>
+    <t>Fletes Carlitos</t>
+  </si>
+  <si>
+    <t>Fecha Prevista</t>
+  </si>
 </sst>
 </file>
 
@@ -319,7 +325,7 @@
     <numFmt numFmtId="165" formatCode="dd\-mm\-yy;@"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -342,8 +348,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="36"/>
+      <name val="Boucherie Block"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -398,8 +414,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFBFBFB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -422,12 +444,108 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -467,9 +585,6 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -479,28 +594,564 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="dd\-mm\-yy;@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="&quot;$&quot;\ #,##0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="dd\-mm\-yy;@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="dd\-mm\-yy;@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFBFBFB"/>
+      <color rgb="FFF7F7F7"/>
+      <color rgb="FFF3F3F3"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -517,15 +1168,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>172720</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>74929</xdr:rowOff>
+      <xdr:rowOff>9526</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>558800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>70380</xdr:rowOff>
+      <xdr:rowOff>193317</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -557,8 +1208,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="172720" y="74929"/>
-          <a:ext cx="3986530" cy="1963951"/>
+          <a:off x="0" y="9526"/>
+          <a:ext cx="11249024" cy="2088791"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -566,13 +1217,7 @@
         <a:ln>
           <a:noFill/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="292100" dist="139700" dir="2700000" algn="tl" rotWithShape="0">
-            <a:srgbClr val="333333">
-              <a:alpha val="65000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:effectLst/>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -669,6 +1314,35 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6F66E3C5-65F7-4FF8-9998-B08288EC3254}" name="Tabla2" displayName="Tabla2" ref="A12:K29" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="13" tableBorderDxfId="14" totalsRowBorderDxfId="12">
+  <autoFilter ref="A12:K29" xr:uid="{6F66E3C5-65F7-4FF8-9998-B08288EC3254}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A13:K29">
+    <sortCondition ref="E12:E29"/>
+  </sortState>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{D559D6D8-6C3E-429F-B747-A4BFA660BC18}" name="Nro Envío" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{693F4542-76CC-4E97-845C-16BA5B020A0B}" name="Fecha de envío" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{8B85FFD0-0538-473C-BCD9-754783EDA3AF}" name="Destino" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{03B91216-44EE-4D64-AFE3-BC57051FE56D}" name="Demora factible" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{0671AD72-17EC-49D9-B177-C24C622DF04E}" name="Fecha de recepcion" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{71E5012F-DBDF-448B-9B38-C63BF73C6450}" name="Costo Flete General" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{78F3F223-DE88-4C63-A248-4FA672E22506}" name="Fecha Prevista" dataDxfId="5">
+      <calculatedColumnFormula>+B13+D13</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{27AF5370-EE83-4026-92E1-19510F15890C}" name="Demora" dataDxfId="4">
+      <calculatedColumnFormula>+IF(E13-G13&lt;=D13,0,E13-G13)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{B0224F9D-6F3B-465A-B5B6-C0B23FD6A049}" name="Entrega_x000a_anticipada" dataDxfId="3">
+      <calculatedColumnFormula>IF(G13&gt;E13,"Si","No")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{08257B80-DCE5-4499-9B41-5A37CB383144}" name="Descuento" dataDxfId="0"/>
+    <tableColumn id="11" xr3:uid="{0F66EA30-29E8-4ED3-BDC9-55F213F6F799}" name="Cobro final" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -968,110 +1642,202 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63EB34BB-64F4-4BD9-8EC3-A6DC807E228F}">
-  <dimension ref="A2:T37"/>
+  <dimension ref="A1:U37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.81640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.453125" style="8" customWidth="1"/>
-    <col min="12" max="16" width="10.90625" style="1"/>
-    <col min="17" max="17" width="31.08984375" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="10.90625" style="1"/>
+    <col min="1" max="1" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.42578125" style="8" customWidth="1"/>
+    <col min="13" max="13" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.85546875" style="1"/>
+    <col min="18" max="18" width="31.140625" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="10.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="7"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="7"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="J4" s="18"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="J5" s="18"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="J6" s="18"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="J7" s="18"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="I11" s="12">
+    <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I1" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="M1" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F2" s="17"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" s="6">
+        <v>2</v>
+      </c>
+      <c r="O2" s="14">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F3" s="17"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="N3" s="6">
+        <v>4</v>
+      </c>
+      <c r="O3" s="14">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="M4" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="6">
+        <v>5</v>
+      </c>
+      <c r="O4" s="14">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="M5" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="N5" s="6">
+        <v>3</v>
+      </c>
+      <c r="O5" s="14">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="M6" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6" s="6">
+        <v>3</v>
+      </c>
+      <c r="O6" s="14">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+    </row>
+    <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="J11" s="12">
         <v>0.03</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="15" t="s">
+    <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="G12" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="H12" s="15" t="s">
+      <c r="I12" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="I12" s="15" t="s">
+      <c r="J12" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="J12" s="15" t="s">
+      <c r="K12" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="K12" s="9"/>
-      <c r="L12" s="21" t="s">
+      <c r="L12" s="9"/>
+      <c r="M12" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="M12" s="21"/>
-      <c r="N12" s="21"/>
-      <c r="O12" s="21"/>
-      <c r="P12" s="21"/>
-      <c r="Q12" s="21"/>
-      <c r="R12" s="21"/>
-      <c r="S12" s="21"/>
-      <c r="T12" s="21"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A13" s="4">
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="19"/>
+      <c r="T12" s="19"/>
+      <c r="U12" s="19"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A13" s="25">
         <v>120035</v>
       </c>
       <c r="B13" s="10">
@@ -1086,25 +1852,38 @@
       <c r="E13" s="10">
         <v>45309</v>
       </c>
-      <c r="F13" s="11"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="L13" s="22" t="s">
+      <c r="F13" s="11">
+        <f>+D13*$O$2</f>
+        <v>5000</v>
+      </c>
+      <c r="G13" s="10">
+        <f>+B13+D13</f>
+        <v>45310</v>
+      </c>
+      <c r="H13" s="28">
+        <f>+IF(E13-G13&lt;=D13,0,E13-G13)</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="27" t="str">
+        <f>IF(G13&gt;E13,"Si","No")</f>
+        <v>Si</v>
+      </c>
+      <c r="J13" s="15"/>
+      <c r="K13" s="29"/>
+      <c r="M13" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="M13" s="22"/>
-      <c r="N13" s="22"/>
-      <c r="O13" s="22"/>
-      <c r="P13" s="22"/>
-      <c r="Q13" s="22"/>
-      <c r="R13" s="22"/>
-      <c r="S13" s="22"/>
-      <c r="T13" s="22"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A14" s="4">
+      <c r="N13" s="20"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="20"/>
+      <c r="Q13" s="20"/>
+      <c r="R13" s="20"/>
+      <c r="S13" s="20"/>
+      <c r="T13" s="20"/>
+      <c r="U13" s="20"/>
+    </row>
+    <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="25">
         <v>120036</v>
       </c>
       <c r="B14" s="10">
@@ -1119,25 +1898,38 @@
       <c r="E14" s="10">
         <v>45313</v>
       </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="L14" s="22" t="s">
+      <c r="F14" s="11">
+        <f>+D14*$O$3</f>
+        <v>12000</v>
+      </c>
+      <c r="G14" s="10">
+        <f>+B14+D14</f>
+        <v>45314</v>
+      </c>
+      <c r="H14" s="28">
+        <f>+IF(E14-G14&lt;=D14,0,E14-G14)</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="27" t="str">
+        <f>IF(G14&gt;E14,"Si","No")</f>
+        <v>Si</v>
+      </c>
+      <c r="J14" s="15"/>
+      <c r="K14" s="29"/>
+      <c r="M14" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="M14" s="22"/>
-      <c r="N14" s="22"/>
-      <c r="O14" s="22"/>
-      <c r="P14" s="22"/>
-      <c r="Q14" s="22"/>
-      <c r="R14" s="22"/>
-      <c r="S14" s="22"/>
-      <c r="T14" s="22"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A15" s="4">
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="20"/>
+      <c r="S14" s="20"/>
+      <c r="T14" s="20"/>
+      <c r="U14" s="20"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A15" s="25">
         <v>120037</v>
       </c>
       <c r="B15" s="10">
@@ -1152,25 +1944,38 @@
       <c r="E15" s="10">
         <v>45340</v>
       </c>
-      <c r="F15" s="11"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="L15" s="22" t="s">
+      <c r="F15" s="11">
+        <f>+D15*$O$4</f>
+        <v>25000</v>
+      </c>
+      <c r="G15" s="10">
+        <f>+B15+D15</f>
+        <v>45315</v>
+      </c>
+      <c r="H15" s="28">
+        <f>+IF(E15-G15&lt;=D15,0,E15-G15)</f>
+        <v>25</v>
+      </c>
+      <c r="I15" s="27" t="str">
+        <f>IF(G15&gt;E15,"Si","No")</f>
+        <v>No</v>
+      </c>
+      <c r="J15" s="15"/>
+      <c r="K15" s="29"/>
+      <c r="M15" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="M15" s="22"/>
-      <c r="N15" s="22"/>
-      <c r="O15" s="22"/>
-      <c r="P15" s="22"/>
-      <c r="Q15" s="22"/>
-      <c r="R15" s="22"/>
-      <c r="S15" s="22"/>
-      <c r="T15" s="22"/>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A16" s="4">
+      <c r="N15" s="20"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="20"/>
+      <c r="Q15" s="20"/>
+      <c r="R15" s="20"/>
+      <c r="S15" s="20"/>
+      <c r="T15" s="20"/>
+      <c r="U15" s="20"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A16" s="25">
         <v>120038</v>
       </c>
       <c r="B16" s="10">
@@ -1185,25 +1990,38 @@
       <c r="E16" s="10">
         <v>45342</v>
       </c>
-      <c r="F16" s="11"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="L16" s="22" t="s">
+      <c r="F16" s="11">
+        <f>+D16*$O$5</f>
+        <v>6000</v>
+      </c>
+      <c r="G16" s="10">
+        <f>+B16+D16</f>
+        <v>45313</v>
+      </c>
+      <c r="H16" s="28">
+        <f>+IF(E16-G16&lt;=D16,0,E16-G16)</f>
+        <v>29</v>
+      </c>
+      <c r="I16" s="27" t="str">
+        <f>IF(G16&gt;E16,"Si","No")</f>
+        <v>No</v>
+      </c>
+      <c r="J16" s="15"/>
+      <c r="K16" s="29"/>
+      <c r="M16" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="M16" s="22"/>
-      <c r="N16" s="22"/>
-      <c r="O16" s="22"/>
-      <c r="P16" s="22"/>
-      <c r="Q16" s="22"/>
-      <c r="R16" s="22"/>
-      <c r="S16" s="22"/>
-      <c r="T16" s="22"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A17" s="4">
+      <c r="N16" s="20"/>
+      <c r="O16" s="20"/>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="20"/>
+      <c r="R16" s="20"/>
+      <c r="S16" s="20"/>
+      <c r="T16" s="20"/>
+      <c r="U16" s="20"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A17" s="25">
         <v>120039</v>
       </c>
       <c r="B17" s="10">
@@ -1218,90 +2036,129 @@
       <c r="E17" s="10">
         <v>45343</v>
       </c>
-      <c r="F17" s="11"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-      <c r="L17" s="22" t="s">
+      <c r="F17" s="11">
+        <f>+D17*$O$5</f>
+        <v>6000</v>
+      </c>
+      <c r="G17" s="10">
+        <f>+B17+D17</f>
+        <v>45314</v>
+      </c>
+      <c r="H17" s="28">
+        <f>+IF(E17-G17&lt;=D17,0,E17-G17)</f>
+        <v>29</v>
+      </c>
+      <c r="I17" s="27" t="str">
+        <f>IF(G17&gt;E17,"Si","No")</f>
+        <v>No</v>
+      </c>
+      <c r="J17" s="15"/>
+      <c r="K17" s="29"/>
+      <c r="M17" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="M17" s="22"/>
-      <c r="N17" s="22"/>
-      <c r="O17" s="22"/>
-      <c r="P17" s="22"/>
-      <c r="Q17" s="22"/>
-      <c r="R17" s="22"/>
-      <c r="S17" s="22"/>
-      <c r="T17" s="22"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A18" s="4">
+      <c r="N17" s="20"/>
+      <c r="O17" s="20"/>
+      <c r="P17" s="20"/>
+      <c r="Q17" s="20"/>
+      <c r="R17" s="20"/>
+      <c r="S17" s="20"/>
+      <c r="T17" s="20"/>
+      <c r="U17" s="20"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A18" s="25">
+        <v>120042</v>
+      </c>
+      <c r="B18" s="10">
+        <v>45315</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="4">
+        <v>4</v>
+      </c>
+      <c r="E18" s="10">
+        <v>45346</v>
+      </c>
+      <c r="F18" s="11">
+        <f>+D18*$O$3</f>
+        <v>12000</v>
+      </c>
+      <c r="G18" s="10">
+        <f>+B18+D18</f>
+        <v>45319</v>
+      </c>
+      <c r="H18" s="28">
+        <f>+IF(E18-G18&lt;=D18,0,E18-G18)</f>
+        <v>27</v>
+      </c>
+      <c r="I18" s="27" t="str">
+        <f>IF(G18&gt;E18,"Si","No")</f>
+        <v>No</v>
+      </c>
+      <c r="J18" s="15"/>
+      <c r="K18" s="29"/>
+      <c r="M18" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="N18" s="20"/>
+      <c r="O18" s="20"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="20"/>
+      <c r="R18" s="20"/>
+      <c r="S18" s="20"/>
+      <c r="T18" s="20"/>
+      <c r="U18" s="20"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A19" s="25">
         <v>120040</v>
-      </c>
-      <c r="B18" s="10">
-        <v>45316</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="4">
-        <v>5</v>
-      </c>
-      <c r="E18" s="10">
-        <v>45347</v>
-      </c>
-      <c r="F18" s="11"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
-      <c r="L18" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="M18" s="22"/>
-      <c r="N18" s="22"/>
-      <c r="O18" s="22"/>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="22"/>
-      <c r="R18" s="22"/>
-      <c r="S18" s="22"/>
-      <c r="T18" s="22"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A19" s="4">
-        <v>120041</v>
       </c>
       <c r="B19" s="10">
         <v>45316</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D19" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E19" s="10">
         <v>45347</v>
       </c>
-      <c r="F19" s="11"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="19"/>
-      <c r="N19" s="19"/>
-      <c r="O19" s="19"/>
-      <c r="P19" s="19"/>
-      <c r="Q19" s="19"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A20" s="4">
-        <v>120042</v>
+      <c r="F19" s="11">
+        <f>+D19*$O$4</f>
+        <v>25000</v>
+      </c>
+      <c r="G19" s="10">
+        <f>+B19+D19</f>
+        <v>45321</v>
+      </c>
+      <c r="H19" s="28">
+        <f>+IF(E19-G19&lt;=D19,0,E19-G19)</f>
+        <v>26</v>
+      </c>
+      <c r="I19" s="27" t="str">
+        <f>IF(G19&gt;E19,"Si","No")</f>
+        <v>No</v>
+      </c>
+      <c r="J19" s="15"/>
+      <c r="K19" s="29"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="22"/>
+      <c r="O19" s="22"/>
+      <c r="P19" s="22"/>
+      <c r="Q19" s="22"/>
+      <c r="R19" s="22"/>
+    </row>
+    <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="25">
+        <v>120041</v>
       </c>
       <c r="B20" s="10">
-        <v>45315</v>
+        <v>45316</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>7</v>
@@ -1310,64 +2167,90 @@
         <v>4</v>
       </c>
       <c r="E20" s="10">
-        <v>45346</v>
-      </c>
-      <c r="F20" s="11"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="16"/>
-      <c r="L20" s="20" t="s">
+        <v>45347</v>
+      </c>
+      <c r="F20" s="11">
+        <f>+D20*$O$3</f>
+        <v>12000</v>
+      </c>
+      <c r="G20" s="10">
+        <f>+B20+D20</f>
+        <v>45320</v>
+      </c>
+      <c r="H20" s="28">
+        <f>+IF(E20-G20&lt;=D20,0,E20-G20)</f>
+        <v>27</v>
+      </c>
+      <c r="I20" s="27" t="str">
+        <f>IF(G20&gt;E20,"Si","No")</f>
+        <v>No</v>
+      </c>
+      <c r="J20" s="15"/>
+      <c r="K20" s="29"/>
+      <c r="M20" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="M20" s="20"/>
-      <c r="N20" s="20"/>
-      <c r="O20" s="20"/>
-      <c r="P20" s="20"/>
-      <c r="Q20" s="20"/>
-      <c r="R20" s="20"/>
-      <c r="S20" s="20"/>
-      <c r="T20" s="20"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A21" s="4">
-        <v>120043</v>
+      <c r="N20" s="18"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="18"/>
+      <c r="Q20" s="18"/>
+      <c r="R20" s="18"/>
+      <c r="S20" s="18"/>
+      <c r="T20" s="18"/>
+      <c r="U20" s="18"/>
+    </row>
+    <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="25">
+        <v>120044</v>
       </c>
       <c r="B21" s="10">
+        <v>45317</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="4">
+        <v>2</v>
+      </c>
+      <c r="E21" s="10">
+        <v>45348</v>
+      </c>
+      <c r="F21" s="11">
+        <f>+D21*$O$2</f>
+        <v>5000</v>
+      </c>
+      <c r="G21" s="10">
+        <f>+B21+D21</f>
+        <v>45319</v>
+      </c>
+      <c r="H21" s="28">
+        <f>+IF(E21-G21&lt;=D21,0,E21-G21)</f>
+        <v>29</v>
+      </c>
+      <c r="I21" s="27" t="str">
+        <f>IF(G21&gt;E21,"Si","No")</f>
+        <v>No</v>
+      </c>
+      <c r="J21" s="15"/>
+      <c r="K21" s="29"/>
+      <c r="M21" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="N21" s="16"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="16"/>
+      <c r="Q21" s="16"/>
+      <c r="R21" s="16"/>
+      <c r="S21" s="16"/>
+      <c r="T21" s="16"/>
+      <c r="U21" s="16"/>
+    </row>
+    <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="25">
+        <v>120045</v>
+      </c>
+      <c r="B22" s="10">
         <v>45318</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="4">
-        <v>4</v>
-      </c>
-      <c r="E21" s="10">
-        <v>45349</v>
-      </c>
-      <c r="F21" s="11"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="L21" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="M21" s="17"/>
-      <c r="N21" s="17"/>
-      <c r="O21" s="17"/>
-      <c r="P21" s="17"/>
-      <c r="Q21" s="17"/>
-      <c r="R21" s="17"/>
-      <c r="S21" s="17"/>
-      <c r="T21" s="17"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A22" s="4">
-        <v>120044</v>
-      </c>
-      <c r="B22" s="10">
-        <v>45317</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>6</v>
@@ -1376,60 +2259,86 @@
         <v>2</v>
       </c>
       <c r="E22" s="10">
-        <v>45348</v>
-      </c>
-      <c r="F22" s="11"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="L22" s="17" t="s">
+        <v>45349</v>
+      </c>
+      <c r="F22" s="11">
+        <f>+D22*$O$2</f>
+        <v>5000</v>
+      </c>
+      <c r="G22" s="10">
+        <f>+B22+D22</f>
+        <v>45320</v>
+      </c>
+      <c r="H22" s="28">
+        <f>+IF(E22-G22&lt;=D22,0,E22-G22)</f>
+        <v>29</v>
+      </c>
+      <c r="I22" s="27" t="str">
+        <f>IF(G22&gt;E22,"Si","No")</f>
+        <v>No</v>
+      </c>
+      <c r="J22" s="15"/>
+      <c r="K22" s="29"/>
+      <c r="M22" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="M22" s="17"/>
-      <c r="N22" s="17"/>
-      <c r="O22" s="17"/>
-      <c r="P22" s="17"/>
-      <c r="Q22" s="17"/>
-      <c r="R22" s="17"/>
-      <c r="S22" s="17"/>
-      <c r="T22" s="17"/>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A23" s="4">
-        <v>120045</v>
+      <c r="N22" s="16"/>
+      <c r="O22" s="16"/>
+      <c r="P22" s="16"/>
+      <c r="Q22" s="16"/>
+      <c r="R22" s="16"/>
+      <c r="S22" s="16"/>
+      <c r="T22" s="16"/>
+      <c r="U22" s="16"/>
+    </row>
+    <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="25">
+        <v>120043</v>
       </c>
       <c r="B23" s="10">
         <v>45318</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D23" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E23" s="10">
         <v>45349</v>
       </c>
-      <c r="F23" s="11"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="L23" s="17" t="s">
+      <c r="F23" s="11">
+        <f>+D23*$O$3</f>
+        <v>12000</v>
+      </c>
+      <c r="G23" s="10">
+        <f>+B23+D23</f>
+        <v>45322</v>
+      </c>
+      <c r="H23" s="28">
+        <f>+IF(E23-G23&lt;=D23,0,E23-G23)</f>
+        <v>27</v>
+      </c>
+      <c r="I23" s="27" t="str">
+        <f>IF(G23&gt;E23,"Si","No")</f>
+        <v>No</v>
+      </c>
+      <c r="J23" s="15"/>
+      <c r="K23" s="29"/>
+      <c r="M23" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="M23" s="17"/>
-      <c r="N23" s="17"/>
-      <c r="O23" s="17"/>
-      <c r="P23" s="17"/>
-      <c r="Q23" s="17"/>
-      <c r="R23" s="17"/>
-      <c r="S23" s="17"/>
-      <c r="T23" s="17"/>
-    </row>
-    <row r="24" spans="1:20" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="4">
+      <c r="N23" s="16"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="16"/>
+      <c r="Q23" s="16"/>
+      <c r="R23" s="16"/>
+      <c r="S23" s="16"/>
+      <c r="T23" s="16"/>
+      <c r="U23" s="16"/>
+    </row>
+    <row r="24" spans="1:21" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="25">
         <v>120046</v>
       </c>
       <c r="B24" s="10">
@@ -1444,25 +2353,38 @@
       <c r="E24" s="10">
         <v>45353</v>
       </c>
-      <c r="F24" s="11"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="L24" s="23" t="s">
+      <c r="F24" s="11">
+        <f>+D24*$O$4</f>
+        <v>25000</v>
+      </c>
+      <c r="G24" s="10">
+        <f>+B24+D24</f>
+        <v>45328</v>
+      </c>
+      <c r="H24" s="28">
+        <f>+IF(E24-G24&lt;=D24,0,E24-G24)</f>
         <v>25</v>
       </c>
-      <c r="M24" s="23"/>
-      <c r="N24" s="23"/>
-      <c r="O24" s="23"/>
-      <c r="P24" s="23"/>
-      <c r="Q24" s="23"/>
-      <c r="R24" s="23"/>
-      <c r="S24" s="23"/>
-      <c r="T24" s="23"/>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A25" s="4">
+      <c r="I24" s="27" t="str">
+        <f>IF(G24&gt;E24,"Si","No")</f>
+        <v>No</v>
+      </c>
+      <c r="J24" s="15"/>
+      <c r="K24" s="29"/>
+      <c r="M24" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="N24" s="21"/>
+      <c r="O24" s="21"/>
+      <c r="P24" s="21"/>
+      <c r="Q24" s="21"/>
+      <c r="R24" s="21"/>
+      <c r="S24" s="21"/>
+      <c r="T24" s="21"/>
+      <c r="U24" s="21"/>
+    </row>
+    <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="25">
         <v>120047</v>
       </c>
       <c r="B25" s="10">
@@ -1477,25 +2399,38 @@
       <c r="E25" s="10">
         <v>45365</v>
       </c>
-      <c r="F25" s="11"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="16"/>
-      <c r="L25" s="17" t="s">
+      <c r="F25" s="11">
+        <f>+D25*$O$4</f>
+        <v>25000</v>
+      </c>
+      <c r="G25" s="10">
+        <f>+B25+D25</f>
+        <v>45329</v>
+      </c>
+      <c r="H25" s="28">
+        <f>+IF(E25-G25&lt;=D25,0,E25-G25)</f>
+        <v>36</v>
+      </c>
+      <c r="I25" s="27" t="str">
+        <f>IF(G25&gt;E25,"Si","No")</f>
+        <v>No</v>
+      </c>
+      <c r="J25" s="15"/>
+      <c r="K25" s="29"/>
+      <c r="M25" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="M25" s="17"/>
-      <c r="N25" s="17"/>
-      <c r="O25" s="17"/>
-      <c r="P25" s="17"/>
-      <c r="Q25" s="17"/>
-      <c r="R25" s="17"/>
-      <c r="S25" s="17"/>
-      <c r="T25" s="17"/>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A26" s="4">
+      <c r="N25" s="16"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="16"/>
+      <c r="Q25" s="16"/>
+      <c r="R25" s="16"/>
+      <c r="S25" s="16"/>
+      <c r="T25" s="16"/>
+      <c r="U25" s="16"/>
+    </row>
+    <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="25">
         <v>120048</v>
       </c>
       <c r="B26" s="10">
@@ -1510,25 +2445,38 @@
       <c r="E26" s="10">
         <v>45382</v>
       </c>
-      <c r="F26" s="11"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
-      <c r="L26" s="17" t="s">
+      <c r="F26" s="11">
+        <f>+D26*$O$6</f>
+        <v>7500</v>
+      </c>
+      <c r="G26" s="10">
+        <f>+B26+D26</f>
+        <v>45325</v>
+      </c>
+      <c r="H26" s="28">
+        <f>+IF(E26-G26&lt;=D26,0,E26-G26)</f>
+        <v>57</v>
+      </c>
+      <c r="I26" s="27" t="str">
+        <f>IF(G26&gt;E26,"Si","No")</f>
+        <v>No</v>
+      </c>
+      <c r="J26" s="15"/>
+      <c r="K26" s="29"/>
+      <c r="M26" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="M26" s="17"/>
-      <c r="N26" s="17"/>
-      <c r="O26" s="17"/>
-      <c r="P26" s="17"/>
-      <c r="Q26" s="17"/>
-      <c r="R26" s="17"/>
-      <c r="S26" s="17"/>
-      <c r="T26" s="17"/>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A27" s="4">
+      <c r="N26" s="16"/>
+      <c r="O26" s="16"/>
+      <c r="P26" s="16"/>
+      <c r="Q26" s="16"/>
+      <c r="R26" s="16"/>
+      <c r="S26" s="16"/>
+      <c r="T26" s="16"/>
+      <c r="U26" s="16"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A27" s="25">
         <v>120049</v>
       </c>
       <c r="B27" s="10">
@@ -1543,25 +2491,38 @@
       <c r="E27" s="10">
         <v>45384</v>
       </c>
-      <c r="F27" s="11"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="16"/>
-      <c r="L27" s="17" t="s">
+      <c r="F27" s="11">
+        <f>+D27*$O$6</f>
+        <v>7500</v>
+      </c>
+      <c r="G27" s="10">
+        <f>+B27+D27</f>
+        <v>45327</v>
+      </c>
+      <c r="H27" s="28">
+        <f>+IF(E27-G27&lt;=D27,0,E27-G27)</f>
+        <v>57</v>
+      </c>
+      <c r="I27" s="27" t="str">
+        <f>IF(G27&gt;E27,"Si","No")</f>
+        <v>No</v>
+      </c>
+      <c r="J27" s="15"/>
+      <c r="K27" s="29"/>
+      <c r="M27" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="M27" s="17"/>
-      <c r="N27" s="17"/>
-      <c r="O27" s="17"/>
-      <c r="P27" s="17"/>
-      <c r="Q27" s="17"/>
-      <c r="R27" s="17"/>
-      <c r="S27" s="17"/>
-      <c r="T27" s="17"/>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A28" s="4">
+      <c r="N27" s="16"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="16"/>
+      <c r="Q27" s="16"/>
+      <c r="R27" s="16"/>
+      <c r="S27" s="16"/>
+      <c r="T27" s="16"/>
+      <c r="U27" s="16"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A28" s="25">
         <v>120050</v>
       </c>
       <c r="B28" s="10">
@@ -1576,82 +2537,109 @@
       <c r="E28" s="10">
         <v>45413</v>
       </c>
-      <c r="F28" s="11"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="16"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A29" s="4">
+      <c r="F28" s="11">
+        <f>+D28*$O$2</f>
+        <v>5000</v>
+      </c>
+      <c r="G28" s="10">
+        <f>+B28+D28</f>
+        <v>45325</v>
+      </c>
+      <c r="H28" s="28">
+        <f>+IF(E28-G28&lt;=D28,0,E28-G28)</f>
+        <v>88</v>
+      </c>
+      <c r="I28" s="27" t="str">
+        <f>IF(G28&gt;E28,"Si","No")</f>
+        <v>No</v>
+      </c>
+      <c r="J28" s="15"/>
+      <c r="K28" s="29"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A29" s="33">
         <v>120051</v>
       </c>
-      <c r="B29" s="10">
+      <c r="B29" s="34">
         <v>45327</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D29" s="35">
         <v>5</v>
       </c>
-      <c r="E29" s="10">
+      <c r="E29" s="34">
         <v>45417</v>
       </c>
-      <c r="F29" s="11"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="F29" s="36">
+        <f>+D29*$O$4</f>
+        <v>25000</v>
+      </c>
+      <c r="G29" s="34">
+        <f>+B29+D29</f>
+        <v>45332</v>
+      </c>
+      <c r="H29" s="37">
+        <f>+IF(E29-G29&lt;=D29,0,E29-G29)</f>
+        <v>85</v>
+      </c>
+      <c r="I29" s="38" t="str">
+        <f>IF(G29&gt;E29,"Si","No")</f>
+        <v>No</v>
+      </c>
+      <c r="J29" s="39"/>
+      <c r="K29" s="40"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="F32" s="2"/>
-    </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="5:9" x14ac:dyDescent="0.2">
       <c r="E33" s="2"/>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="5:9" x14ac:dyDescent="0.2">
       <c r="E34" s="2"/>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="5:9" x14ac:dyDescent="0.2">
       <c r="E35" s="2"/>
-    </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="I35" s="24"/>
+    </row>
+    <row r="36" spans="5:9" x14ac:dyDescent="0.2">
       <c r="E36" s="2"/>
     </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="5:9" x14ac:dyDescent="0.2">
       <c r="E37" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="L27:T27"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="L21:T21"/>
-    <mergeCell ref="L22:T22"/>
-    <mergeCell ref="L23:T23"/>
-    <mergeCell ref="L20:T20"/>
-    <mergeCell ref="L12:T12"/>
-    <mergeCell ref="L13:T13"/>
-    <mergeCell ref="L14:T14"/>
-    <mergeCell ref="L15:T15"/>
-    <mergeCell ref="L16:T16"/>
-    <mergeCell ref="L17:T17"/>
-    <mergeCell ref="L18:T18"/>
-    <mergeCell ref="L24:T24"/>
-    <mergeCell ref="L25:T25"/>
-    <mergeCell ref="L26:T26"/>
+  <mergeCells count="19">
+    <mergeCell ref="M26:U26"/>
     <mergeCell ref="F2:F3"/>
-    <mergeCell ref="L19:Q19"/>
-    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="M19:R19"/>
     <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="I1:K10"/>
+    <mergeCell ref="M27:U27"/>
+    <mergeCell ref="M21:U21"/>
+    <mergeCell ref="M22:U22"/>
+    <mergeCell ref="M23:U23"/>
+    <mergeCell ref="M20:U20"/>
+    <mergeCell ref="M12:U12"/>
+    <mergeCell ref="M13:U13"/>
+    <mergeCell ref="M14:U14"/>
+    <mergeCell ref="M15:U15"/>
+    <mergeCell ref="M16:U16"/>
+    <mergeCell ref="M17:U17"/>
+    <mergeCell ref="M18:U18"/>
+    <mergeCell ref="M24:U24"/>
+    <mergeCell ref="M25:U25"/>
   </mergeCells>
   <pageMargins left="0.74803149606299213" right="0.74803149606299213" top="0.98425196850393704" bottom="0.98425196850393704" header="0" footer="0"/>
   <pageSetup scale="77" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1660,16 +2648,16 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C6" sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
@@ -1680,7 +2668,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
@@ -1691,7 +2679,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -1702,7 +2690,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>8</v>
       </c>
@@ -1713,7 +2701,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
@@ -1724,7 +2712,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>14</v>
       </c>
@@ -1735,7 +2723,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -2181,15 +3169,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Teams_Channel_Section_Location xmlns="dcd687b3-ff2a-4cef-8a8e-ae79212dfc5f" xsi:nil="true"/>
@@ -2242,6 +3221,15 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{909C7340-0040-4780-BC94-6D84F39177D5}">
   <ds:schemaRefs>
@@ -2262,14 +3250,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{260CA9CC-D738-4B67-AAAD-54E1EF5E89C7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EE0433A-D7D3-4596-A96A-E3E9D5FA36B9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -2284,4 +3264,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{260CA9CC-D738-4B67-AAAD-54E1EF5E89C7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>